<commit_message>
Removed the spaced between trials in the data csv
</commit_message>
<xml_diff>
--- a/preamp_data.xlsx
+++ b/preamp_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nova\Desktop\School\Current Semester\PHYS_4007 Fourth Year Physics Lab\lockinAmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9C91ED1-B2D6-4F8F-8C3B-134C84B639DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6398013C-AACA-4F39-9FE0-5472B9D2113C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{144EF43C-66E9-41CF-97DB-62E0FCF5D54F}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CDA341B-3BF6-4C69-8345-06E2EEAC2785}">
-  <dimension ref="A1:D176"/>
+  <dimension ref="A1:D169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="A180" sqref="A180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,12 +670,26 @@
         <v>-8.5000000000000006E-3</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="D20">
+        <v>-1.4E-2</v>
+      </c>
+    </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C21">
         <v>1.4800000000000001E-2</v>
@@ -689,7 +703,7 @@
         <v>2</v>
       </c>
       <c r="B22">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C22">
         <v>1.4800000000000001E-2</v>
@@ -703,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="B23">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="C23">
         <v>1.4800000000000001E-2</v>
@@ -717,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="C24">
         <v>1.4800000000000001E-2</v>
@@ -731,7 +745,7 @@
         <v>2</v>
       </c>
       <c r="B25">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C25">
         <v>1.4800000000000001E-2</v>
@@ -745,7 +759,7 @@
         <v>2</v>
       </c>
       <c r="B26">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="C26">
         <v>1.4800000000000001E-2</v>
@@ -759,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="B27">
-        <v>5000</v>
+        <v>7500</v>
       </c>
       <c r="C27">
         <v>1.4800000000000001E-2</v>
@@ -773,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="B28">
-        <v>7500</v>
+        <v>10000</v>
       </c>
       <c r="C28">
         <v>1.4800000000000001E-2</v>
@@ -787,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="B29">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="C29">
         <v>1.4800000000000001E-2</v>
@@ -801,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="B30">
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="C30">
         <v>1.4800000000000001E-2</v>
@@ -815,7 +829,7 @@
         <v>2</v>
       </c>
       <c r="B31">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="C31">
         <v>1.4800000000000001E-2</v>
@@ -829,7 +843,7 @@
         <v>2</v>
       </c>
       <c r="B32">
-        <v>50000</v>
+        <v>75000</v>
       </c>
       <c r="C32">
         <v>1.4800000000000001E-2</v>
@@ -843,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="B33">
-        <v>75000</v>
+        <v>100000</v>
       </c>
       <c r="C33">
         <v>1.4800000000000001E-2</v>
@@ -857,13 +871,13 @@
         <v>2</v>
       </c>
       <c r="B34">
-        <v>100000</v>
+        <v>300000</v>
       </c>
       <c r="C34">
-        <v>1.4800000000000001E-2</v>
+        <v>1.8800000000000001E-2</v>
       </c>
       <c r="D34">
-        <v>-1.4E-2</v>
+        <v>-1.6E-2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -871,13 +885,13 @@
         <v>2</v>
       </c>
       <c r="B35">
-        <v>300000</v>
+        <v>500000</v>
       </c>
       <c r="C35">
-        <v>1.8800000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D35">
-        <v>-1.6E-2</v>
+        <v>-1.84E-2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -885,13 +899,13 @@
         <v>2</v>
       </c>
       <c r="B36">
-        <v>500000</v>
+        <v>750000</v>
       </c>
       <c r="C36">
-        <v>0.02</v>
+        <v>1.6400000000000001E-2</v>
       </c>
       <c r="D36">
-        <v>-1.84E-2</v>
+        <v>-1.4200000000000001E-2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -899,27 +913,41 @@
         <v>2</v>
       </c>
       <c r="B37">
-        <v>750000</v>
+        <v>1000000</v>
       </c>
       <c r="C37">
-        <v>1.6400000000000001E-2</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="D37">
-        <v>-1.4200000000000001E-2</v>
+        <v>-1.06E-2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B38">
-        <v>1000000</v>
+        <v>20</v>
       </c>
       <c r="C38">
-        <v>1.2800000000000001E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="D38">
-        <v>-1.06E-2</v>
+        <v>-2.4E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>100</v>
+      </c>
+      <c r="C39">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D39">
+        <v>-2.4E-2</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -927,13 +955,13 @@
         <v>5</v>
       </c>
       <c r="B40">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="C40">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="D40">
-        <v>-2.4E-2</v>
+        <v>-2.4799999999999999E-2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -941,13 +969,13 @@
         <v>5</v>
       </c>
       <c r="B41">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="C41">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="D41">
-        <v>-2.4E-2</v>
+        <v>-2.4799999999999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -955,7 +983,7 @@
         <v>5</v>
       </c>
       <c r="B42">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="C42">
         <v>3.7999999999999999E-2</v>
@@ -969,10 +997,10 @@
         <v>5</v>
       </c>
       <c r="B43">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="C43">
-        <v>3.7999999999999999E-2</v>
+        <v>2.9600000000000001E-2</v>
       </c>
       <c r="D43">
         <v>-2.4799999999999999E-2</v>
@@ -983,10 +1011,10 @@
         <v>5</v>
       </c>
       <c r="B44">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="C44">
-        <v>3.7999999999999999E-2</v>
+        <v>2.9600000000000001E-2</v>
       </c>
       <c r="D44">
         <v>-2.4799999999999999E-2</v>
@@ -997,7 +1025,7 @@
         <v>5</v>
       </c>
       <c r="B45">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="C45">
         <v>2.9600000000000001E-2</v>
@@ -1011,7 +1039,7 @@
         <v>5</v>
       </c>
       <c r="B46">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="C46">
         <v>2.9600000000000001E-2</v>
@@ -1025,7 +1053,7 @@
         <v>5</v>
       </c>
       <c r="B47">
-        <v>7500</v>
+        <v>15000</v>
       </c>
       <c r="C47">
         <v>2.9600000000000001E-2</v>
@@ -1039,7 +1067,7 @@
         <v>5</v>
       </c>
       <c r="B48">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="C48">
         <v>2.9600000000000001E-2</v>
@@ -1053,7 +1081,7 @@
         <v>5</v>
       </c>
       <c r="B49">
-        <v>15000</v>
+        <v>50000</v>
       </c>
       <c r="C49">
         <v>2.9600000000000001E-2</v>
@@ -1067,7 +1095,7 @@
         <v>5</v>
       </c>
       <c r="B50">
-        <v>20000</v>
+        <v>75000</v>
       </c>
       <c r="C50">
         <v>2.9600000000000001E-2</v>
@@ -1081,7 +1109,7 @@
         <v>5</v>
       </c>
       <c r="B51">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="C51">
         <v>2.9600000000000001E-2</v>
@@ -1095,13 +1123,13 @@
         <v>5</v>
       </c>
       <c r="B52">
-        <v>75000</v>
+        <v>300000</v>
       </c>
       <c r="C52">
-        <v>2.9600000000000001E-2</v>
+        <v>3.32E-2</v>
       </c>
       <c r="D52">
-        <v>-2.4799999999999999E-2</v>
+        <v>-2.8400000000000002E-2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1109,13 +1137,13 @@
         <v>5</v>
       </c>
       <c r="B53">
-        <v>100000</v>
+        <v>500000</v>
       </c>
       <c r="C53">
-        <v>2.9600000000000001E-2</v>
+        <v>3.5200000000000002E-2</v>
       </c>
       <c r="D53">
-        <v>-2.4799999999999999E-2</v>
+        <v>-2.9600000000000001E-2</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1123,13 +1151,13 @@
         <v>5</v>
       </c>
       <c r="B54">
-        <v>300000</v>
+        <v>600000</v>
       </c>
       <c r="C54">
-        <v>3.32E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="D54">
-        <v>-2.8400000000000002E-2</v>
+        <v>-2.52E-2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1137,13 +1165,13 @@
         <v>5</v>
       </c>
       <c r="B55">
-        <v>500000</v>
+        <v>700000</v>
       </c>
       <c r="C55">
-        <v>3.5200000000000002E-2</v>
+        <v>2.76E-2</v>
       </c>
       <c r="D55">
-        <v>-2.9600000000000001E-2</v>
+        <v>-2.0799999999999999E-2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1151,13 +1179,13 @@
         <v>5</v>
       </c>
       <c r="B56">
-        <v>600000</v>
+        <v>750000</v>
       </c>
       <c r="C56">
-        <v>3.2000000000000001E-2</v>
+        <v>2.5600000000000001E-2</v>
       </c>
       <c r="D56">
-        <v>-2.52E-2</v>
+        <v>-1.9199999999999998E-2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1165,13 +1193,13 @@
         <v>5</v>
       </c>
       <c r="B57">
-        <v>700000</v>
+        <v>800000</v>
       </c>
       <c r="C57">
-        <v>2.76E-2</v>
+        <v>2.3199999999999998E-2</v>
       </c>
       <c r="D57">
-        <v>-2.0799999999999999E-2</v>
+        <v>-1.72E-2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1179,13 +1207,13 @@
         <v>5</v>
       </c>
       <c r="B58">
-        <v>750000</v>
+        <v>900000</v>
       </c>
       <c r="C58">
-        <v>2.5600000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D58">
-        <v>-1.9199999999999998E-2</v>
+        <v>-1.44E-2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1193,41 +1221,55 @@
         <v>5</v>
       </c>
       <c r="B59">
-        <v>800000</v>
+        <v>1000000</v>
       </c>
       <c r="C59">
-        <v>2.3199999999999998E-2</v>
+        <v>1.8800000000000001E-2</v>
       </c>
       <c r="D59">
-        <v>-1.72E-2</v>
+        <v>-1.2800000000000001E-2</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B60">
-        <v>900000</v>
+        <v>20</v>
       </c>
       <c r="C60">
-        <v>0.02</v>
+        <v>5.6800000000000003E-2</v>
       </c>
       <c r="D60">
-        <v>-1.44E-2</v>
+        <v>-4.5199999999999997E-2</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B61">
-        <v>1000000</v>
+        <v>100</v>
       </c>
       <c r="C61">
-        <v>1.8800000000000001E-2</v>
+        <v>5.6800000000000003E-2</v>
       </c>
       <c r="D61">
-        <v>-1.2800000000000001E-2</v>
+        <v>-4.5199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>10</v>
+      </c>
+      <c r="B62">
+        <v>200</v>
+      </c>
+      <c r="C62">
+        <v>5.6800000000000003E-2</v>
+      </c>
+      <c r="D62">
+        <v>-4.5199999999999997E-2</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1235,7 +1277,7 @@
         <v>10</v>
       </c>
       <c r="B63">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="C63">
         <v>5.6800000000000003E-2</v>
@@ -1249,7 +1291,7 @@
         <v>10</v>
       </c>
       <c r="B64">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C64">
         <v>5.6800000000000003E-2</v>
@@ -1263,7 +1305,7 @@
         <v>10</v>
       </c>
       <c r="B65">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="C65">
         <v>5.6800000000000003E-2</v>
@@ -1277,7 +1319,7 @@
         <v>10</v>
       </c>
       <c r="B66">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="C66">
         <v>5.6800000000000003E-2</v>
@@ -1291,13 +1333,13 @@
         <v>10</v>
       </c>
       <c r="B67">
-        <v>1000</v>
+        <v>7500</v>
       </c>
       <c r="C67">
         <v>5.6800000000000003E-2</v>
       </c>
       <c r="D67">
-        <v>-4.5199999999999997E-2</v>
+        <v>-4.4400000000000002E-2</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1305,13 +1347,13 @@
         <v>10</v>
       </c>
       <c r="B68">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="C68">
         <v>5.6800000000000003E-2</v>
       </c>
       <c r="D68">
-        <v>-4.5199999999999997E-2</v>
+        <v>-4.4400000000000002E-2</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1319,13 +1361,13 @@
         <v>10</v>
       </c>
       <c r="B69">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="C69">
         <v>5.6800000000000003E-2</v>
       </c>
       <c r="D69">
-        <v>-4.5199999999999997E-2</v>
+        <v>-4.4400000000000002E-2</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1333,7 +1375,7 @@
         <v>10</v>
       </c>
       <c r="B70">
-        <v>7500</v>
+        <v>20000</v>
       </c>
       <c r="C70">
         <v>5.6800000000000003E-2</v>
@@ -1347,7 +1389,7 @@
         <v>10</v>
       </c>
       <c r="B71">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="C71">
         <v>5.6800000000000003E-2</v>
@@ -1361,7 +1403,7 @@
         <v>10</v>
       </c>
       <c r="B72">
-        <v>15000</v>
+        <v>75000</v>
       </c>
       <c r="C72">
         <v>5.6800000000000003E-2</v>
@@ -1375,13 +1417,13 @@
         <v>10</v>
       </c>
       <c r="B73">
-        <v>20000</v>
+        <v>100000</v>
       </c>
       <c r="C73">
-        <v>5.6800000000000003E-2</v>
+        <v>5.7200000000000001E-2</v>
       </c>
       <c r="D73">
-        <v>-4.4400000000000002E-2</v>
+        <v>-4.48E-2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1389,13 +1431,13 @@
         <v>10</v>
       </c>
       <c r="B74">
-        <v>50000</v>
+        <v>300000</v>
       </c>
       <c r="C74">
-        <v>5.6800000000000003E-2</v>
+        <v>5.96E-2</v>
       </c>
       <c r="D74">
-        <v>-4.4400000000000002E-2</v>
+        <v>-4.7600000000000003E-2</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1403,13 +1445,13 @@
         <v>10</v>
       </c>
       <c r="B75">
-        <v>75000</v>
+        <v>500000</v>
       </c>
       <c r="C75">
-        <v>5.6800000000000003E-2</v>
+        <v>5.28E-2</v>
       </c>
       <c r="D75">
-        <v>-4.4400000000000002E-2</v>
+        <v>-4.1200000000000001E-2</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1417,13 +1459,13 @@
         <v>10</v>
       </c>
       <c r="B76">
-        <v>100000</v>
+        <v>600000</v>
       </c>
       <c r="C76">
-        <v>5.7200000000000001E-2</v>
+        <v>4.6800000000000001E-2</v>
       </c>
       <c r="D76">
-        <v>-4.48E-2</v>
+        <v>-3.4000000000000002E-2</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1431,13 +1473,13 @@
         <v>10</v>
       </c>
       <c r="B77">
-        <v>300000</v>
+        <v>700000</v>
       </c>
       <c r="C77">
-        <v>5.96E-2</v>
+        <v>3.8800000000000001E-2</v>
       </c>
       <c r="D77">
-        <v>-4.7600000000000003E-2</v>
+        <v>-2.64E-2</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1445,13 +1487,13 @@
         <v>10</v>
       </c>
       <c r="B78">
-        <v>500000</v>
+        <v>750000</v>
       </c>
       <c r="C78">
-        <v>5.28E-2</v>
+        <v>3.6600000000000001E-2</v>
       </c>
       <c r="D78">
-        <v>-4.1200000000000001E-2</v>
+        <v>-2.3599999999999999E-2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1459,13 +1501,13 @@
         <v>10</v>
       </c>
       <c r="B79">
-        <v>600000</v>
+        <v>800000</v>
       </c>
       <c r="C79">
-        <v>4.6800000000000001E-2</v>
+        <v>3.32E-2</v>
       </c>
       <c r="D79">
-        <v>-3.4000000000000002E-2</v>
+        <v>-2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1473,13 +1515,13 @@
         <v>10</v>
       </c>
       <c r="B80">
-        <v>700000</v>
+        <v>900000</v>
       </c>
       <c r="C80">
-        <v>3.8800000000000001E-2</v>
+        <v>2.92E-2</v>
       </c>
       <c r="D80">
-        <v>-2.64E-2</v>
+        <v>-1.6799999999999999E-2</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1487,55 +1529,69 @@
         <v>10</v>
       </c>
       <c r="B81">
-        <v>750000</v>
+        <v>1000000</v>
       </c>
       <c r="C81">
-        <v>3.6600000000000001E-2</v>
+        <v>2.6200000000000001E-2</v>
       </c>
       <c r="D81">
-        <v>-2.3599999999999999E-2</v>
+        <v>-1.3599999999999999E-2</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B82">
-        <v>800000</v>
+        <v>20</v>
       </c>
       <c r="C82">
-        <v>3.32E-2</v>
+        <v>0.112</v>
       </c>
       <c r="D82">
-        <v>-2.1000000000000001E-2</v>
+        <v>-8.5999999999999993E-2</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B83">
-        <v>900000</v>
+        <v>100</v>
       </c>
       <c r="C83">
-        <v>2.92E-2</v>
+        <v>0.112</v>
       </c>
       <c r="D83">
-        <v>-1.6799999999999999E-2</v>
+        <v>-8.5999999999999993E-2</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B84">
-        <v>1000000</v>
+        <v>200</v>
       </c>
       <c r="C84">
-        <v>2.6200000000000001E-2</v>
+        <v>0.112</v>
       </c>
       <c r="D84">
-        <v>-1.3599999999999999E-2</v>
+        <v>-8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>20</v>
+      </c>
+      <c r="B85">
+        <v>500</v>
+      </c>
+      <c r="C85">
+        <v>0.112</v>
+      </c>
+      <c r="D85">
+        <v>-8.7999999999999995E-2</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1543,13 +1599,13 @@
         <v>20</v>
       </c>
       <c r="B86">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="C86">
         <v>0.112</v>
       </c>
       <c r="D86">
-        <v>-8.5999999999999993E-2</v>
+        <v>-8.7999999999999995E-2</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1557,13 +1613,13 @@
         <v>20</v>
       </c>
       <c r="B87">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="C87">
         <v>0.112</v>
       </c>
       <c r="D87">
-        <v>-8.5999999999999993E-2</v>
+        <v>-8.7999999999999995E-2</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1571,13 +1627,13 @@
         <v>20</v>
       </c>
       <c r="B88">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="C88">
         <v>0.112</v>
       </c>
       <c r="D88">
-        <v>-8.5999999999999993E-2</v>
+        <v>-8.7999999999999995E-2</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1585,7 +1641,7 @@
         <v>20</v>
       </c>
       <c r="B89">
-        <v>500</v>
+        <v>7500</v>
       </c>
       <c r="C89">
         <v>0.112</v>
@@ -1599,7 +1655,7 @@
         <v>20</v>
       </c>
       <c r="B90">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="C90">
         <v>0.112</v>
@@ -1613,7 +1669,7 @@
         <v>20</v>
       </c>
       <c r="B91">
-        <v>2000</v>
+        <v>15000</v>
       </c>
       <c r="C91">
         <v>0.112</v>
@@ -1627,7 +1683,7 @@
         <v>20</v>
       </c>
       <c r="B92">
-        <v>5000</v>
+        <v>20000</v>
       </c>
       <c r="C92">
         <v>0.112</v>
@@ -1641,7 +1697,7 @@
         <v>20</v>
       </c>
       <c r="B93">
-        <v>7500</v>
+        <v>50000</v>
       </c>
       <c r="C93">
         <v>0.112</v>
@@ -1655,7 +1711,7 @@
         <v>20</v>
       </c>
       <c r="B94">
-        <v>10000</v>
+        <v>75000</v>
       </c>
       <c r="C94">
         <v>0.112</v>
@@ -1669,7 +1725,7 @@
         <v>20</v>
       </c>
       <c r="B95">
-        <v>15000</v>
+        <v>100000</v>
       </c>
       <c r="C95">
         <v>0.112</v>
@@ -1683,13 +1739,13 @@
         <v>20</v>
       </c>
       <c r="B96">
-        <v>20000</v>
+        <v>300000</v>
       </c>
       <c r="C96">
-        <v>0.112</v>
+        <v>0.104</v>
       </c>
       <c r="D96">
-        <v>-8.7999999999999995E-2</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1697,13 +1753,13 @@
         <v>20</v>
       </c>
       <c r="B97">
-        <v>50000</v>
+        <v>400000</v>
       </c>
       <c r="C97">
-        <v>0.112</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="D97">
-        <v>-8.7999999999999995E-2</v>
+        <v>-6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1711,13 +1767,13 @@
         <v>20</v>
       </c>
       <c r="B98">
-        <v>75000</v>
+        <v>500000</v>
       </c>
       <c r="C98">
-        <v>0.112</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="D98">
-        <v>-8.7999999999999995E-2</v>
+        <v>-5.5E-2</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1725,13 +1781,13 @@
         <v>20</v>
       </c>
       <c r="B99">
-        <v>100000</v>
+        <v>600000</v>
       </c>
       <c r="C99">
-        <v>0.112</v>
+        <v>6.5600000000000006E-2</v>
       </c>
       <c r="D99">
-        <v>-8.7999999999999995E-2</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -1739,13 +1795,13 @@
         <v>20</v>
       </c>
       <c r="B100">
-        <v>300000</v>
+        <v>700000</v>
       </c>
       <c r="C100">
-        <v>0.104</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="D100">
-        <v>-0.08</v>
+        <v>-3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1753,13 +1809,13 @@
         <v>20</v>
       </c>
       <c r="B101">
-        <v>400000</v>
+        <v>750000</v>
       </c>
       <c r="C101">
-        <v>9.2999999999999999E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="D101">
-        <v>-6.8000000000000005E-2</v>
+        <v>-2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -1767,13 +1823,13 @@
         <v>20</v>
       </c>
       <c r="B102">
-        <v>500000</v>
+        <v>800000</v>
       </c>
       <c r="C102">
-        <v>7.9000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D102">
-        <v>-5.5E-2</v>
+        <v>-2.4E-2</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -1781,13 +1837,13 @@
         <v>20</v>
       </c>
       <c r="B103">
-        <v>600000</v>
+        <v>900000</v>
       </c>
       <c r="C103">
-        <v>6.5600000000000006E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D103">
-        <v>-0.04</v>
+        <v>-1.9E-2</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -1795,69 +1851,83 @@
         <v>20</v>
       </c>
       <c r="B104">
-        <v>700000</v>
+        <v>1000000</v>
       </c>
       <c r="C104">
-        <v>5.7000000000000002E-2</v>
+        <v>0.04</v>
       </c>
       <c r="D104">
-        <v>-3.2000000000000001E-2</v>
+        <v>-1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B105">
-        <v>750000</v>
+        <v>20</v>
       </c>
       <c r="C105">
-        <v>5.3999999999999999E-2</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="D105">
-        <v>-2.9000000000000001E-2</v>
+        <v>-0.214</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B106">
-        <v>800000</v>
+        <v>100</v>
       </c>
       <c r="C106">
-        <v>0.05</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="D106">
-        <v>-2.4E-2</v>
+        <v>-0.214</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B107">
-        <v>900000</v>
+        <v>200</v>
       </c>
       <c r="C107">
-        <v>4.4999999999999998E-2</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="D107">
-        <v>-1.9E-2</v>
+        <v>-0.214</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B108">
-        <v>1000000</v>
+        <v>500</v>
       </c>
       <c r="C108">
-        <v>0.04</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="D108">
-        <v>-1.4999999999999999E-2</v>
+        <v>-0.214</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>50</v>
+      </c>
+      <c r="B109">
+        <v>1000</v>
+      </c>
+      <c r="C109">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="D109">
+        <v>-0.214</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -1865,13 +1935,13 @@
         <v>50</v>
       </c>
       <c r="B110">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="C110">
-        <v>0.27800000000000002</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D110">
-        <v>-0.214</v>
+        <v>-0.21199999999999999</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -1879,13 +1949,13 @@
         <v>50</v>
       </c>
       <c r="B111">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="C111">
-        <v>0.27800000000000002</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D111">
-        <v>-0.214</v>
+        <v>-0.21199999999999999</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -1893,13 +1963,13 @@
         <v>50</v>
       </c>
       <c r="B112">
-        <v>200</v>
+        <v>7500</v>
       </c>
       <c r="C112">
-        <v>0.27800000000000002</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D112">
-        <v>-0.214</v>
+        <v>-0.21199999999999999</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -1907,13 +1977,13 @@
         <v>50</v>
       </c>
       <c r="B113">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="C113">
-        <v>0.27800000000000002</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D113">
-        <v>-0.214</v>
+        <v>-0.21199999999999999</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -1921,13 +1991,13 @@
         <v>50</v>
       </c>
       <c r="B114">
-        <v>1000</v>
+        <v>15000</v>
       </c>
       <c r="C114">
-        <v>0.27800000000000002</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="D114">
-        <v>-0.214</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -1935,13 +2005,13 @@
         <v>50</v>
       </c>
       <c r="B115">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="C115">
-        <v>0.28000000000000003</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="D115">
-        <v>-0.21199999999999999</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -1949,13 +2019,13 @@
         <v>50</v>
       </c>
       <c r="B116">
-        <v>5000</v>
+        <v>50000</v>
       </c>
       <c r="C116">
-        <v>0.28000000000000003</v>
+        <v>0.27</v>
       </c>
       <c r="D116">
-        <v>-0.21199999999999999</v>
+        <v>-0.20399999999999999</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -1963,13 +2033,13 @@
         <v>50</v>
       </c>
       <c r="B117">
-        <v>7500</v>
+        <v>75000</v>
       </c>
       <c r="C117">
-        <v>0.28000000000000003</v>
+        <v>0.26600000000000001</v>
       </c>
       <c r="D117">
-        <v>-0.21199999999999999</v>
+        <v>-0.19600000000000001</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -1977,13 +2047,13 @@
         <v>50</v>
       </c>
       <c r="B118">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="C118">
-        <v>0.28000000000000003</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="D118">
-        <v>-0.21199999999999999</v>
+        <v>-0.19</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -1991,13 +2061,13 @@
         <v>50</v>
       </c>
       <c r="B119">
-        <v>15000</v>
+        <v>200000</v>
       </c>
       <c r="C119">
-        <v>0.27600000000000002</v>
+        <v>0.20799999999999999</v>
       </c>
       <c r="D119">
-        <v>-0.21</v>
+        <v>-0.14599999999999999</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2005,13 +2075,13 @@
         <v>50</v>
       </c>
       <c r="B120">
-        <v>20000</v>
+        <v>300000</v>
       </c>
       <c r="C120">
-        <v>0.27600000000000002</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="D120">
-        <v>-0.21</v>
+        <v>-0.105</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2019,13 +2089,13 @@
         <v>50</v>
       </c>
       <c r="B121">
-        <v>50000</v>
+        <v>400000</v>
       </c>
       <c r="C121">
-        <v>0.27</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="D121">
-        <v>-0.20399999999999999</v>
+        <v>-7.2999999999999995E-2</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2033,13 +2103,13 @@
         <v>50</v>
       </c>
       <c r="B122">
-        <v>75000</v>
+        <v>500000</v>
       </c>
       <c r="C122">
-        <v>0.26600000000000001</v>
+        <v>0.113</v>
       </c>
       <c r="D122">
-        <v>-0.19600000000000001</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2047,13 +2117,13 @@
         <v>50</v>
       </c>
       <c r="B123">
-        <v>100000</v>
+        <v>600000</v>
       </c>
       <c r="C123">
-        <v>0.25600000000000001</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="D123">
-        <v>-0.19</v>
+        <v>-3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2061,13 +2131,13 @@
         <v>50</v>
       </c>
       <c r="B124">
-        <v>200000</v>
+        <v>700000</v>
       </c>
       <c r="C124">
-        <v>0.20799999999999999</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="D124">
-        <v>-0.14599999999999999</v>
+        <v>-2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2075,13 +2145,13 @@
         <v>50</v>
       </c>
       <c r="B125">
-        <v>300000</v>
+        <v>750000</v>
       </c>
       <c r="C125">
-        <v>0.16700000000000001</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="D125">
-        <v>-0.105</v>
+        <v>-1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2089,13 +2159,13 @@
         <v>50</v>
       </c>
       <c r="B126">
-        <v>400000</v>
+        <v>800000</v>
       </c>
       <c r="C126">
-        <v>0.13600000000000001</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="D126">
-        <v>-7.2999999999999995E-2</v>
+        <v>-1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2103,13 +2173,13 @@
         <v>50</v>
       </c>
       <c r="B127">
-        <v>500000</v>
+        <v>900000</v>
       </c>
       <c r="C127">
-        <v>0.113</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="D127">
-        <v>-0.05</v>
+        <v>-6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2117,83 +2187,97 @@
         <v>50</v>
       </c>
       <c r="B128">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="C128">
-        <v>9.8000000000000004E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="D128">
-        <v>-3.3000000000000002E-2</v>
+        <v>-2E-3</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B129">
-        <v>700000</v>
+        <v>20</v>
       </c>
       <c r="C129">
-        <v>8.6999999999999994E-2</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="D129">
-        <v>-2.1999999999999999E-2</v>
+        <v>-0.41599999999999998</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B130">
-        <v>750000</v>
+        <v>100</v>
       </c>
       <c r="C130">
-        <v>8.2000000000000003E-2</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="D130">
-        <v>-1.7000000000000001E-2</v>
+        <v>-0.42</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B131">
-        <v>800000</v>
+        <v>200</v>
       </c>
       <c r="C131">
-        <v>7.9000000000000001E-2</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="D131">
-        <v>-1.2999999999999999E-2</v>
+        <v>-0.42</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B132">
-        <v>900000</v>
+        <v>500</v>
       </c>
       <c r="C132">
-        <v>7.1999999999999995E-2</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="D132">
-        <v>-6.0000000000000001E-3</v>
+        <v>-0.42</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B133">
-        <v>1000000</v>
+        <v>1000</v>
       </c>
       <c r="C133">
-        <v>6.7000000000000004E-2</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="D133">
-        <v>-2E-3</v>
+        <v>-0.42399999999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>100</v>
+      </c>
+      <c r="B134">
+        <v>2000</v>
+      </c>
+      <c r="C134">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="D134">
+        <v>-0.42399999999999999</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -2201,13 +2285,13 @@
         <v>100</v>
       </c>
       <c r="B135">
-        <v>20</v>
+        <v>5000</v>
       </c>
       <c r="C135">
         <v>0.54400000000000004</v>
       </c>
       <c r="D135">
-        <v>-0.41599999999999998</v>
+        <v>-0.42399999999999999</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -2215,13 +2299,13 @@
         <v>100</v>
       </c>
       <c r="B136">
-        <v>100</v>
+        <v>7500</v>
       </c>
       <c r="C136">
-        <v>0.54800000000000004</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="D136">
-        <v>-0.42</v>
+        <v>-0.42399999999999999</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -2229,10 +2313,10 @@
         <v>100</v>
       </c>
       <c r="B137">
-        <v>200</v>
+        <v>10000</v>
       </c>
       <c r="C137">
-        <v>0.54800000000000004</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="D137">
         <v>-0.42</v>
@@ -2243,10 +2327,10 @@
         <v>100</v>
       </c>
       <c r="B138">
-        <v>500</v>
+        <v>15000</v>
       </c>
       <c r="C138">
-        <v>0.54800000000000004</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="D138">
         <v>-0.42</v>
@@ -2257,13 +2341,13 @@
         <v>100</v>
       </c>
       <c r="B139">
-        <v>1000</v>
+        <v>20000</v>
       </c>
       <c r="C139">
-        <v>0.54400000000000004</v>
+        <v>0.54</v>
       </c>
       <c r="D139">
-        <v>-0.42399999999999999</v>
+        <v>-0.41199999999999998</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -2271,13 +2355,13 @@
         <v>100</v>
       </c>
       <c r="B140">
-        <v>2000</v>
+        <v>50000</v>
       </c>
       <c r="C140">
-        <v>0.54400000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="D140">
-        <v>-0.42399999999999999</v>
+        <v>-0.376</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -2285,13 +2369,13 @@
         <v>100</v>
       </c>
       <c r="B141">
-        <v>5000</v>
+        <v>75000</v>
       </c>
       <c r="C141">
-        <v>0.54400000000000004</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="D141">
-        <v>-0.42399999999999999</v>
+        <v>-0.33200000000000002</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -2299,13 +2383,13 @@
         <v>100</v>
       </c>
       <c r="B142">
-        <v>7500</v>
+        <v>100000</v>
       </c>
       <c r="C142">
-        <v>0.54400000000000004</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="D142">
-        <v>-0.42399999999999999</v>
+        <v>-0.28799999999999998</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -2313,13 +2397,13 @@
         <v>100</v>
       </c>
       <c r="B143">
-        <v>10000</v>
+        <v>150000</v>
       </c>
       <c r="C143">
-        <v>0.54400000000000004</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="D143">
-        <v>-0.42</v>
+        <v>-0.216</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -2327,13 +2411,13 @@
         <v>100</v>
       </c>
       <c r="B144">
-        <v>15000</v>
+        <v>200000</v>
       </c>
       <c r="C144">
-        <v>0.54400000000000004</v>
+        <v>0.29199999999999998</v>
       </c>
       <c r="D144">
-        <v>-0.42</v>
+        <v>-0.16400000000000001</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -2341,13 +2425,13 @@
         <v>100</v>
       </c>
       <c r="B145">
-        <v>20000</v>
+        <v>300000</v>
       </c>
       <c r="C145">
-        <v>0.54</v>
+        <v>0.22</v>
       </c>
       <c r="D145">
-        <v>-0.41199999999999998</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -2355,13 +2439,13 @@
         <v>100</v>
       </c>
       <c r="B146">
-        <v>50000</v>
+        <v>500000</v>
       </c>
       <c r="C146">
-        <v>0.5</v>
+        <v>0.156</v>
       </c>
       <c r="D146">
-        <v>-0.376</v>
+        <v>-2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -2369,13 +2453,13 @@
         <v>100</v>
       </c>
       <c r="B147">
-        <v>75000</v>
+        <v>600000</v>
       </c>
       <c r="C147">
-        <v>0.45600000000000002</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="D147">
-        <v>-0.33200000000000002</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -2383,13 +2467,13 @@
         <v>100</v>
       </c>
       <c r="B148">
-        <v>100000</v>
+        <v>700000</v>
       </c>
       <c r="C148">
-        <v>0.41599999999999998</v>
+        <v>0.124</v>
       </c>
       <c r="D148">
-        <v>-0.28799999999999998</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -2397,97 +2481,111 @@
         <v>100</v>
       </c>
       <c r="B149">
-        <v>150000</v>
+        <v>1000000</v>
       </c>
       <c r="C149">
-        <v>0.34799999999999998</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="D149">
-        <v>-0.216</v>
+        <v>2.7E-2</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B150">
-        <v>200000</v>
+        <v>20</v>
       </c>
       <c r="C150">
-        <v>0.29199999999999998</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D150">
-        <v>-0.16400000000000001</v>
+        <v>-0.84</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B151">
-        <v>300000</v>
+        <v>100</v>
       </c>
       <c r="C151">
-        <v>0.22</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D151">
-        <v>-0.09</v>
+        <v>-0.85</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B152">
-        <v>500000</v>
+        <v>200</v>
       </c>
       <c r="C152">
-        <v>0.156</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D152">
-        <v>-2.5999999999999999E-2</v>
+        <v>-0.85</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B153">
-        <v>600000</v>
+        <v>500</v>
       </c>
       <c r="C153">
-        <v>0.13400000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D153">
-        <v>-8.0000000000000002E-3</v>
+        <v>-0.85</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B154">
-        <v>700000</v>
+        <v>1000</v>
       </c>
       <c r="C154">
-        <v>0.124</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D154">
-        <v>5.0000000000000001E-3</v>
+        <v>-0.85</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B155">
-        <v>1000000</v>
+        <v>2000</v>
       </c>
       <c r="C155">
-        <v>0.10299999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="D155">
-        <v>2.7E-2</v>
+        <v>-0.87</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>200</v>
+      </c>
+      <c r="B156">
+        <v>5000</v>
+      </c>
+      <c r="C156">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="D156">
+        <v>-0.87</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -2495,13 +2593,13 @@
         <v>200</v>
       </c>
       <c r="B157">
-        <v>20</v>
+        <v>7500</v>
       </c>
       <c r="C157">
-        <v>1.1000000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="D157">
-        <v>-0.84</v>
+        <v>-0.87</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -2509,7 +2607,7 @@
         <v>200</v>
       </c>
       <c r="B158">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="C158">
         <v>1.1000000000000001</v>
@@ -2523,13 +2621,13 @@
         <v>200</v>
       </c>
       <c r="B159">
-        <v>200</v>
+        <v>15000</v>
       </c>
       <c r="C159">
-        <v>1.1000000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="D159">
-        <v>-0.85</v>
+        <v>-0.82</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -2537,13 +2635,13 @@
         <v>200</v>
       </c>
       <c r="B160">
-        <v>500</v>
+        <v>20000</v>
       </c>
       <c r="C160">
-        <v>1.1000000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="D160">
-        <v>-0.85</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -2551,13 +2649,13 @@
         <v>200</v>
       </c>
       <c r="B161">
-        <v>1000</v>
+        <v>30000</v>
       </c>
       <c r="C161">
-        <v>1.1000000000000001</v>
+        <v>0.98</v>
       </c>
       <c r="D161">
-        <v>-0.85</v>
+        <v>-0.73</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -2565,13 +2663,13 @@
         <v>200</v>
       </c>
       <c r="B162">
-        <v>2000</v>
+        <v>40000</v>
       </c>
       <c r="C162">
-        <v>1.1200000000000001</v>
+        <v>0.91</v>
       </c>
       <c r="D162">
-        <v>-0.87</v>
+        <v>-0.65</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -2579,13 +2677,13 @@
         <v>200</v>
       </c>
       <c r="B163">
-        <v>5000</v>
+        <v>50000</v>
       </c>
       <c r="C163">
-        <v>1.1200000000000001</v>
+        <v>0.85</v>
       </c>
       <c r="D163">
-        <v>-0.87</v>
+        <v>-0.59</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -2593,13 +2691,13 @@
         <v>200</v>
       </c>
       <c r="B164">
-        <v>7500</v>
+        <v>75000</v>
       </c>
       <c r="C164">
-        <v>1.1200000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="D164">
-        <v>-0.87</v>
+        <v>-0.44</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -2607,13 +2705,13 @@
         <v>200</v>
       </c>
       <c r="B165">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="C165">
-        <v>1.1000000000000001</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D165">
-        <v>-0.85</v>
+        <v>-0.32400000000000001</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -2621,13 +2719,13 @@
         <v>200</v>
       </c>
       <c r="B166">
-        <v>15000</v>
+        <v>200000</v>
       </c>
       <c r="C166">
-        <v>1.08</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="D166">
-        <v>-0.82</v>
+        <v>-0.124</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -2635,13 +2733,13 @@
         <v>200</v>
       </c>
       <c r="B167">
-        <v>20000</v>
+        <v>500000</v>
       </c>
       <c r="C167">
-        <v>1.05</v>
+        <v>0.224</v>
       </c>
       <c r="D167">
-        <v>-0.8</v>
+        <v>3.4000000000000002E-2</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -2649,13 +2747,13 @@
         <v>200</v>
       </c>
       <c r="B168">
-        <v>30000</v>
+        <v>700000</v>
       </c>
       <c r="C168">
-        <v>0.98</v>
+        <v>0.2</v>
       </c>
       <c r="D168">
-        <v>-0.73</v>
+        <v>6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -2663,110 +2761,12 @@
         <v>200</v>
       </c>
       <c r="B169">
-        <v>40000</v>
+        <v>1000000</v>
       </c>
       <c r="C169">
-        <v>0.91</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="D169">
-        <v>-0.65</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170">
-        <v>200</v>
-      </c>
-      <c r="B170">
-        <v>50000</v>
-      </c>
-      <c r="C170">
-        <v>0.85</v>
-      </c>
-      <c r="D170">
-        <v>-0.59</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171">
-        <v>200</v>
-      </c>
-      <c r="B171">
-        <v>75000</v>
-      </c>
-      <c r="C171">
-        <v>0.7</v>
-      </c>
-      <c r="D171">
-        <v>-0.44</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172">
-        <v>200</v>
-      </c>
-      <c r="B172">
-        <v>100000</v>
-      </c>
-      <c r="C172">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="D172">
-        <v>-0.32400000000000001</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173">
-        <v>200</v>
-      </c>
-      <c r="B173">
-        <v>200000</v>
-      </c>
-      <c r="C173">
-        <v>0.38400000000000001</v>
-      </c>
-      <c r="D173">
-        <v>-0.124</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174">
-        <v>200</v>
-      </c>
-      <c r="B174">
-        <v>500000</v>
-      </c>
-      <c r="C174">
-        <v>0.224</v>
-      </c>
-      <c r="D174">
-        <v>3.4000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175">
-        <v>200</v>
-      </c>
-      <c r="B175">
-        <v>700000</v>
-      </c>
-      <c r="C175">
-        <v>0.2</v>
-      </c>
-      <c r="D175">
-        <v>6.8000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176">
-        <v>200</v>
-      </c>
-      <c r="B176">
-        <v>1000000</v>
-      </c>
-      <c r="C176">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="D176">
         <v>8.8999999999999996E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated data to have latest trials preamp_analysis works with 3dB scatter point for each trial.
</commit_message>
<xml_diff>
--- a/preamp_data.xlsx
+++ b/preamp_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nova\Desktop\School\Current Semester\PHYS_4007 Fourth Year Physics Lab\lockinAmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6398013C-AACA-4F39-9FE0-5472B9D2113C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B82E34-6E14-438A-98B3-CCC4071103DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{144EF43C-66E9-41CF-97DB-62E0FCF5D54F}"/>
   </bookViews>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CDA341B-3BF6-4C69-8345-06E2EEAC2785}">
-  <dimension ref="A1:D169"/>
+  <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="A180" sqref="A180"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A172" sqref="A172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,30 +672,30 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20">
-        <v>20</v>
+        <v>1500000</v>
       </c>
       <c r="C20">
-        <v>1.4800000000000001E-2</v>
+        <v>7.4000000000000003E-3</v>
       </c>
       <c r="D20">
-        <v>-1.4E-2</v>
+        <v>-6.1999999999999998E-3</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21">
-        <v>100</v>
+        <v>2000000</v>
       </c>
       <c r="C21">
-        <v>1.4800000000000001E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="D21">
-        <v>-1.4E-2</v>
+        <v>-4.4000000000000003E-3</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -703,7 +703,7 @@
         <v>2</v>
       </c>
       <c r="B22">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="C22">
         <v>1.4800000000000001E-2</v>
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="B23">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="C23">
         <v>1.4800000000000001E-2</v>
@@ -731,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="C24">
         <v>1.4800000000000001E-2</v>
@@ -745,7 +745,7 @@
         <v>2</v>
       </c>
       <c r="B25">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="C25">
         <v>1.4800000000000001E-2</v>
@@ -759,7 +759,7 @@
         <v>2</v>
       </c>
       <c r="B26">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="C26">
         <v>1.4800000000000001E-2</v>
@@ -773,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="B27">
-        <v>7500</v>
+        <v>2000</v>
       </c>
       <c r="C27">
         <v>1.4800000000000001E-2</v>
@@ -787,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="B28">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="C28">
         <v>1.4800000000000001E-2</v>
@@ -801,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="B29">
-        <v>15000</v>
+        <v>7500</v>
       </c>
       <c r="C29">
         <v>1.4800000000000001E-2</v>
@@ -815,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="B30">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="C30">
         <v>1.4800000000000001E-2</v>
@@ -829,7 +829,7 @@
         <v>2</v>
       </c>
       <c r="B31">
-        <v>50000</v>
+        <v>15000</v>
       </c>
       <c r="C31">
         <v>1.4800000000000001E-2</v>
@@ -843,7 +843,7 @@
         <v>2</v>
       </c>
       <c r="B32">
-        <v>75000</v>
+        <v>20000</v>
       </c>
       <c r="C32">
         <v>1.4800000000000001E-2</v>
@@ -857,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="B33">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="C33">
         <v>1.4800000000000001E-2</v>
@@ -871,13 +871,13 @@
         <v>2</v>
       </c>
       <c r="B34">
-        <v>300000</v>
+        <v>75000</v>
       </c>
       <c r="C34">
-        <v>1.8800000000000001E-2</v>
+        <v>1.4800000000000001E-2</v>
       </c>
       <c r="D34">
-        <v>-1.6E-2</v>
+        <v>-1.4E-2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -885,13 +885,13 @@
         <v>2</v>
       </c>
       <c r="B35">
-        <v>500000</v>
+        <v>100000</v>
       </c>
       <c r="C35">
-        <v>0.02</v>
+        <v>1.4800000000000001E-2</v>
       </c>
       <c r="D35">
-        <v>-1.84E-2</v>
+        <v>-1.4E-2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -899,13 +899,13 @@
         <v>2</v>
       </c>
       <c r="B36">
-        <v>750000</v>
+        <v>300000</v>
       </c>
       <c r="C36">
-        <v>1.6400000000000001E-2</v>
+        <v>1.8800000000000001E-2</v>
       </c>
       <c r="D36">
-        <v>-1.4200000000000001E-2</v>
+        <v>-1.6E-2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -913,55 +913,55 @@
         <v>2</v>
       </c>
       <c r="B37">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="C37">
-        <v>1.2800000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D37">
-        <v>-1.06E-2</v>
+        <v>-1.84E-2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B38">
-        <v>20</v>
+        <v>750000</v>
       </c>
       <c r="C38">
-        <v>3.7999999999999999E-2</v>
+        <v>1.6400000000000001E-2</v>
       </c>
       <c r="D38">
-        <v>-2.4E-2</v>
+        <v>-1.4200000000000001E-2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B39">
-        <v>100</v>
+        <v>1000000</v>
       </c>
       <c r="C39">
-        <v>3.7999999999999999E-2</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="D39">
-        <v>-2.4E-2</v>
+        <v>-1.06E-2</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B40">
-        <v>200</v>
+        <v>1500000</v>
       </c>
       <c r="C40">
-        <v>3.7999999999999999E-2</v>
+        <v>8.2000000000000007E-3</v>
       </c>
       <c r="D40">
-        <v>-2.4799999999999999E-2</v>
+        <v>-5.7999999999999996E-3</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -969,13 +969,13 @@
         <v>5</v>
       </c>
       <c r="B41">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="C41">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="D41">
-        <v>-2.4799999999999999E-2</v>
+        <v>-2.4E-2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -983,13 +983,13 @@
         <v>5</v>
       </c>
       <c r="B42">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C42">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="D42">
-        <v>-2.4799999999999999E-2</v>
+        <v>-2.4E-2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -997,10 +997,10 @@
         <v>5</v>
       </c>
       <c r="B43">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="C43">
-        <v>2.9600000000000001E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="D43">
         <v>-2.4799999999999999E-2</v>
@@ -1011,10 +1011,10 @@
         <v>5</v>
       </c>
       <c r="B44">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="C44">
-        <v>2.9600000000000001E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="D44">
         <v>-2.4799999999999999E-2</v>
@@ -1025,10 +1025,10 @@
         <v>5</v>
       </c>
       <c r="B45">
-        <v>7500</v>
+        <v>1000</v>
       </c>
       <c r="C45">
-        <v>2.9600000000000001E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="D45">
         <v>-2.4799999999999999E-2</v>
@@ -1039,7 +1039,7 @@
         <v>5</v>
       </c>
       <c r="B46">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="C46">
         <v>2.9600000000000001E-2</v>
@@ -1053,7 +1053,7 @@
         <v>5</v>
       </c>
       <c r="B47">
-        <v>15000</v>
+        <v>5000</v>
       </c>
       <c r="C47">
         <v>2.9600000000000001E-2</v>
@@ -1067,7 +1067,7 @@
         <v>5</v>
       </c>
       <c r="B48">
-        <v>20000</v>
+        <v>7500</v>
       </c>
       <c r="C48">
         <v>2.9600000000000001E-2</v>
@@ -1081,7 +1081,7 @@
         <v>5</v>
       </c>
       <c r="B49">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="C49">
         <v>2.9600000000000001E-2</v>
@@ -1095,7 +1095,7 @@
         <v>5</v>
       </c>
       <c r="B50">
-        <v>75000</v>
+        <v>15000</v>
       </c>
       <c r="C50">
         <v>2.9600000000000001E-2</v>
@@ -1109,7 +1109,7 @@
         <v>5</v>
       </c>
       <c r="B51">
-        <v>100000</v>
+        <v>20000</v>
       </c>
       <c r="C51">
         <v>2.9600000000000001E-2</v>
@@ -1123,13 +1123,13 @@
         <v>5</v>
       </c>
       <c r="B52">
-        <v>300000</v>
+        <v>50000</v>
       </c>
       <c r="C52">
-        <v>3.32E-2</v>
+        <v>2.9600000000000001E-2</v>
       </c>
       <c r="D52">
-        <v>-2.8400000000000002E-2</v>
+        <v>-2.4799999999999999E-2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1137,13 +1137,13 @@
         <v>5</v>
       </c>
       <c r="B53">
-        <v>500000</v>
+        <v>75000</v>
       </c>
       <c r="C53">
-        <v>3.5200000000000002E-2</v>
+        <v>2.9600000000000001E-2</v>
       </c>
       <c r="D53">
-        <v>-2.9600000000000001E-2</v>
+        <v>-2.4799999999999999E-2</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1151,13 +1151,13 @@
         <v>5</v>
       </c>
       <c r="B54">
-        <v>600000</v>
+        <v>100000</v>
       </c>
       <c r="C54">
-        <v>3.2000000000000001E-2</v>
+        <v>2.9600000000000001E-2</v>
       </c>
       <c r="D54">
-        <v>-2.52E-2</v>
+        <v>-2.4799999999999999E-2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1165,13 +1165,13 @@
         <v>5</v>
       </c>
       <c r="B55">
-        <v>700000</v>
+        <v>300000</v>
       </c>
       <c r="C55">
-        <v>2.76E-2</v>
+        <v>3.32E-2</v>
       </c>
       <c r="D55">
-        <v>-2.0799999999999999E-2</v>
+        <v>-2.8400000000000002E-2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1179,13 +1179,13 @@
         <v>5</v>
       </c>
       <c r="B56">
-        <v>750000</v>
+        <v>500000</v>
       </c>
       <c r="C56">
-        <v>2.5600000000000001E-2</v>
+        <v>3.5200000000000002E-2</v>
       </c>
       <c r="D56">
-        <v>-1.9199999999999998E-2</v>
+        <v>-2.9600000000000001E-2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1193,13 +1193,13 @@
         <v>5</v>
       </c>
       <c r="B57">
-        <v>800000</v>
+        <v>600000</v>
       </c>
       <c r="C57">
-        <v>2.3199999999999998E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="D57">
-        <v>-1.72E-2</v>
+        <v>-2.52E-2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1207,13 +1207,13 @@
         <v>5</v>
       </c>
       <c r="B58">
-        <v>900000</v>
+        <v>700000</v>
       </c>
       <c r="C58">
-        <v>0.02</v>
+        <v>2.76E-2</v>
       </c>
       <c r="D58">
-        <v>-1.44E-2</v>
+        <v>-2.0799999999999999E-2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1221,55 +1221,55 @@
         <v>5</v>
       </c>
       <c r="B59">
-        <v>1000000</v>
+        <v>750000</v>
       </c>
       <c r="C59">
-        <v>1.8800000000000001E-2</v>
+        <v>2.5600000000000001E-2</v>
       </c>
       <c r="D59">
-        <v>-1.2800000000000001E-2</v>
+        <v>-1.9199999999999998E-2</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B60">
-        <v>20</v>
+        <v>800000</v>
       </c>
       <c r="C60">
-        <v>5.6800000000000003E-2</v>
+        <v>2.3199999999999998E-2</v>
       </c>
       <c r="D60">
-        <v>-4.5199999999999997E-2</v>
+        <v>-1.72E-2</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B61">
-        <v>100</v>
+        <v>900000</v>
       </c>
       <c r="C61">
-        <v>5.6800000000000003E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D61">
-        <v>-4.5199999999999997E-2</v>
+        <v>-1.44E-2</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B62">
-        <v>200</v>
+        <v>1000000</v>
       </c>
       <c r="C62">
-        <v>5.6800000000000003E-2</v>
+        <v>1.8800000000000001E-2</v>
       </c>
       <c r="D62">
-        <v>-4.5199999999999997E-2</v>
+        <v>-1.2800000000000001E-2</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1277,7 +1277,7 @@
         <v>10</v>
       </c>
       <c r="B63">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="C63">
         <v>5.6800000000000003E-2</v>
@@ -1291,7 +1291,7 @@
         <v>10</v>
       </c>
       <c r="B64">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C64">
         <v>5.6800000000000003E-2</v>
@@ -1305,7 +1305,7 @@
         <v>10</v>
       </c>
       <c r="B65">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="C65">
         <v>5.6800000000000003E-2</v>
@@ -1319,7 +1319,7 @@
         <v>10</v>
       </c>
       <c r="B66">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="C66">
         <v>5.6800000000000003E-2</v>
@@ -1333,13 +1333,13 @@
         <v>10</v>
       </c>
       <c r="B67">
-        <v>7500</v>
+        <v>1000</v>
       </c>
       <c r="C67">
         <v>5.6800000000000003E-2</v>
       </c>
       <c r="D67">
-        <v>-4.4400000000000002E-2</v>
+        <v>-4.5199999999999997E-2</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1347,13 +1347,13 @@
         <v>10</v>
       </c>
       <c r="B68">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="C68">
         <v>5.6800000000000003E-2</v>
       </c>
       <c r="D68">
-        <v>-4.4400000000000002E-2</v>
+        <v>-4.5199999999999997E-2</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1361,13 +1361,13 @@
         <v>10</v>
       </c>
       <c r="B69">
-        <v>15000</v>
+        <v>5000</v>
       </c>
       <c r="C69">
         <v>5.6800000000000003E-2</v>
       </c>
       <c r="D69">
-        <v>-4.4400000000000002E-2</v>
+        <v>-4.5199999999999997E-2</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1375,7 +1375,7 @@
         <v>10</v>
       </c>
       <c r="B70">
-        <v>20000</v>
+        <v>7500</v>
       </c>
       <c r="C70">
         <v>5.6800000000000003E-2</v>
@@ -1389,7 +1389,7 @@
         <v>10</v>
       </c>
       <c r="B71">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="C71">
         <v>5.6800000000000003E-2</v>
@@ -1403,7 +1403,7 @@
         <v>10</v>
       </c>
       <c r="B72">
-        <v>75000</v>
+        <v>15000</v>
       </c>
       <c r="C72">
         <v>5.6800000000000003E-2</v>
@@ -1417,13 +1417,13 @@
         <v>10</v>
       </c>
       <c r="B73">
-        <v>100000</v>
+        <v>20000</v>
       </c>
       <c r="C73">
-        <v>5.7200000000000001E-2</v>
+        <v>5.6800000000000003E-2</v>
       </c>
       <c r="D73">
-        <v>-4.48E-2</v>
+        <v>-4.4400000000000002E-2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1431,13 +1431,13 @@
         <v>10</v>
       </c>
       <c r="B74">
-        <v>300000</v>
+        <v>50000</v>
       </c>
       <c r="C74">
-        <v>5.96E-2</v>
+        <v>5.6800000000000003E-2</v>
       </c>
       <c r="D74">
-        <v>-4.7600000000000003E-2</v>
+        <v>-4.4400000000000002E-2</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1445,13 +1445,13 @@
         <v>10</v>
       </c>
       <c r="B75">
-        <v>500000</v>
+        <v>75000</v>
       </c>
       <c r="C75">
-        <v>5.28E-2</v>
+        <v>5.6800000000000003E-2</v>
       </c>
       <c r="D75">
-        <v>-4.1200000000000001E-2</v>
+        <v>-4.4400000000000002E-2</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1459,13 +1459,13 @@
         <v>10</v>
       </c>
       <c r="B76">
-        <v>600000</v>
+        <v>100000</v>
       </c>
       <c r="C76">
-        <v>4.6800000000000001E-2</v>
+        <v>5.7200000000000001E-2</v>
       </c>
       <c r="D76">
-        <v>-3.4000000000000002E-2</v>
+        <v>-4.48E-2</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1473,13 +1473,13 @@
         <v>10</v>
       </c>
       <c r="B77">
-        <v>700000</v>
+        <v>300000</v>
       </c>
       <c r="C77">
-        <v>3.8800000000000001E-2</v>
+        <v>5.96E-2</v>
       </c>
       <c r="D77">
-        <v>-2.64E-2</v>
+        <v>-4.7600000000000003E-2</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1487,13 +1487,13 @@
         <v>10</v>
       </c>
       <c r="B78">
-        <v>750000</v>
+        <v>500000</v>
       </c>
       <c r="C78">
-        <v>3.6600000000000001E-2</v>
+        <v>5.28E-2</v>
       </c>
       <c r="D78">
-        <v>-2.3599999999999999E-2</v>
+        <v>-4.1200000000000001E-2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1501,13 +1501,13 @@
         <v>10</v>
       </c>
       <c r="B79">
-        <v>800000</v>
+        <v>600000</v>
       </c>
       <c r="C79">
-        <v>3.32E-2</v>
+        <v>4.6800000000000001E-2</v>
       </c>
       <c r="D79">
-        <v>-2.1000000000000001E-2</v>
+        <v>-3.4000000000000002E-2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1515,13 +1515,13 @@
         <v>10</v>
       </c>
       <c r="B80">
-        <v>900000</v>
+        <v>700000</v>
       </c>
       <c r="C80">
-        <v>2.92E-2</v>
+        <v>3.8800000000000001E-2</v>
       </c>
       <c r="D80">
-        <v>-1.6799999999999999E-2</v>
+        <v>-2.64E-2</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1529,55 +1529,55 @@
         <v>10</v>
       </c>
       <c r="B81">
-        <v>1000000</v>
+        <v>750000</v>
       </c>
       <c r="C81">
-        <v>2.6200000000000001E-2</v>
+        <v>3.6600000000000001E-2</v>
       </c>
       <c r="D81">
-        <v>-1.3599999999999999E-2</v>
+        <v>-2.3599999999999999E-2</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B82">
-        <v>20</v>
+        <v>800000</v>
       </c>
       <c r="C82">
-        <v>0.112</v>
+        <v>3.32E-2</v>
       </c>
       <c r="D82">
-        <v>-8.5999999999999993E-2</v>
+        <v>-2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B83">
-        <v>100</v>
+        <v>900000</v>
       </c>
       <c r="C83">
-        <v>0.112</v>
+        <v>2.92E-2</v>
       </c>
       <c r="D83">
-        <v>-8.5999999999999993E-2</v>
+        <v>-1.6799999999999999E-2</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B84">
-        <v>200</v>
+        <v>1000000</v>
       </c>
       <c r="C84">
-        <v>0.112</v>
+        <v>2.6200000000000001E-2</v>
       </c>
       <c r="D84">
-        <v>-8.5999999999999993E-2</v>
+        <v>-1.3599999999999999E-2</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1585,13 +1585,13 @@
         <v>20</v>
       </c>
       <c r="B85">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="C85">
         <v>0.112</v>
       </c>
       <c r="D85">
-        <v>-8.7999999999999995E-2</v>
+        <v>-8.5999999999999993E-2</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1599,13 +1599,13 @@
         <v>20</v>
       </c>
       <c r="B86">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C86">
         <v>0.112</v>
       </c>
       <c r="D86">
-        <v>-8.7999999999999995E-2</v>
+        <v>-8.5999999999999993E-2</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1613,13 +1613,13 @@
         <v>20</v>
       </c>
       <c r="B87">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="C87">
         <v>0.112</v>
       </c>
       <c r="D87">
-        <v>-8.7999999999999995E-2</v>
+        <v>-8.5999999999999993E-2</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1627,7 +1627,7 @@
         <v>20</v>
       </c>
       <c r="B88">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="C88">
         <v>0.112</v>
@@ -1641,7 +1641,7 @@
         <v>20</v>
       </c>
       <c r="B89">
-        <v>7500</v>
+        <v>1000</v>
       </c>
       <c r="C89">
         <v>0.112</v>
@@ -1655,7 +1655,7 @@
         <v>20</v>
       </c>
       <c r="B90">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="C90">
         <v>0.112</v>
@@ -1669,7 +1669,7 @@
         <v>20</v>
       </c>
       <c r="B91">
-        <v>15000</v>
+        <v>5000</v>
       </c>
       <c r="C91">
         <v>0.112</v>
@@ -1683,7 +1683,7 @@
         <v>20</v>
       </c>
       <c r="B92">
-        <v>20000</v>
+        <v>7500</v>
       </c>
       <c r="C92">
         <v>0.112</v>
@@ -1697,7 +1697,7 @@
         <v>20</v>
       </c>
       <c r="B93">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="C93">
         <v>0.112</v>
@@ -1711,7 +1711,7 @@
         <v>20</v>
       </c>
       <c r="B94">
-        <v>75000</v>
+        <v>15000</v>
       </c>
       <c r="C94">
         <v>0.112</v>
@@ -1725,7 +1725,7 @@
         <v>20</v>
       </c>
       <c r="B95">
-        <v>100000</v>
+        <v>20000</v>
       </c>
       <c r="C95">
         <v>0.112</v>
@@ -1739,13 +1739,13 @@
         <v>20</v>
       </c>
       <c r="B96">
-        <v>300000</v>
+        <v>50000</v>
       </c>
       <c r="C96">
-        <v>0.104</v>
+        <v>0.112</v>
       </c>
       <c r="D96">
-        <v>-0.08</v>
+        <v>-8.7999999999999995E-2</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1753,13 +1753,13 @@
         <v>20</v>
       </c>
       <c r="B97">
-        <v>400000</v>
+        <v>75000</v>
       </c>
       <c r="C97">
-        <v>9.2999999999999999E-2</v>
+        <v>0.112</v>
       </c>
       <c r="D97">
-        <v>-6.8000000000000005E-2</v>
+        <v>-8.7999999999999995E-2</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1767,13 +1767,13 @@
         <v>20</v>
       </c>
       <c r="B98">
-        <v>500000</v>
+        <v>100000</v>
       </c>
       <c r="C98">
-        <v>7.9000000000000001E-2</v>
+        <v>0.112</v>
       </c>
       <c r="D98">
-        <v>-5.5E-2</v>
+        <v>-8.7999999999999995E-2</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1781,13 +1781,13 @@
         <v>20</v>
       </c>
       <c r="B99">
-        <v>600000</v>
+        <v>300000</v>
       </c>
       <c r="C99">
-        <v>6.5600000000000006E-2</v>
+        <v>0.104</v>
       </c>
       <c r="D99">
-        <v>-0.04</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -1795,13 +1795,13 @@
         <v>20</v>
       </c>
       <c r="B100">
-        <v>700000</v>
+        <v>400000</v>
       </c>
       <c r="C100">
-        <v>5.7000000000000002E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="D100">
-        <v>-3.2000000000000001E-2</v>
+        <v>-6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1809,13 +1809,13 @@
         <v>20</v>
       </c>
       <c r="B101">
-        <v>750000</v>
+        <v>500000</v>
       </c>
       <c r="C101">
-        <v>5.3999999999999999E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="D101">
-        <v>-2.9000000000000001E-2</v>
+        <v>-5.5E-2</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -1823,13 +1823,13 @@
         <v>20</v>
       </c>
       <c r="B102">
-        <v>800000</v>
+        <v>600000</v>
       </c>
       <c r="C102">
-        <v>0.05</v>
+        <v>6.5600000000000006E-2</v>
       </c>
       <c r="D102">
-        <v>-2.4E-2</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -1837,13 +1837,13 @@
         <v>20</v>
       </c>
       <c r="B103">
-        <v>900000</v>
+        <v>700000</v>
       </c>
       <c r="C103">
-        <v>4.4999999999999998E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="D103">
-        <v>-1.9E-2</v>
+        <v>-3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -1851,55 +1851,55 @@
         <v>20</v>
       </c>
       <c r="B104">
-        <v>1000000</v>
+        <v>750000</v>
       </c>
       <c r="C104">
-        <v>0.04</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="D104">
-        <v>-1.4999999999999999E-2</v>
+        <v>-2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B105">
-        <v>20</v>
+        <v>800000</v>
       </c>
       <c r="C105">
-        <v>0.27800000000000002</v>
+        <v>0.05</v>
       </c>
       <c r="D105">
-        <v>-0.214</v>
+        <v>-2.4E-2</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B106">
-        <v>100</v>
+        <v>900000</v>
       </c>
       <c r="C106">
-        <v>0.27800000000000002</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D106">
-        <v>-0.214</v>
+        <v>-1.9E-2</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B107">
-        <v>200</v>
+        <v>1000000</v>
       </c>
       <c r="C107">
-        <v>0.27800000000000002</v>
+        <v>0.04</v>
       </c>
       <c r="D107">
-        <v>-0.214</v>
+        <v>-1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -1907,7 +1907,7 @@
         <v>50</v>
       </c>
       <c r="B108">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="C108">
         <v>0.27800000000000002</v>
@@ -1921,7 +1921,7 @@
         <v>50</v>
       </c>
       <c r="B109">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C109">
         <v>0.27800000000000002</v>
@@ -1935,13 +1935,13 @@
         <v>50</v>
       </c>
       <c r="B110">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="C110">
-        <v>0.28000000000000003</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="D110">
-        <v>-0.21199999999999999</v>
+        <v>-0.214</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -1949,13 +1949,13 @@
         <v>50</v>
       </c>
       <c r="B111">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="C111">
-        <v>0.28000000000000003</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="D111">
-        <v>-0.21199999999999999</v>
+        <v>-0.214</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -1963,13 +1963,13 @@
         <v>50</v>
       </c>
       <c r="B112">
-        <v>7500</v>
+        <v>1000</v>
       </c>
       <c r="C112">
-        <v>0.28000000000000003</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="D112">
-        <v>-0.21199999999999999</v>
+        <v>-0.214</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -1977,7 +1977,7 @@
         <v>50</v>
       </c>
       <c r="B113">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="C113">
         <v>0.28000000000000003</v>
@@ -1991,13 +1991,13 @@
         <v>50</v>
       </c>
       <c r="B114">
-        <v>15000</v>
+        <v>5000</v>
       </c>
       <c r="C114">
-        <v>0.27600000000000002</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D114">
-        <v>-0.21</v>
+        <v>-0.21199999999999999</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2005,13 +2005,13 @@
         <v>50</v>
       </c>
       <c r="B115">
-        <v>20000</v>
+        <v>7500</v>
       </c>
       <c r="C115">
-        <v>0.27600000000000002</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D115">
-        <v>-0.21</v>
+        <v>-0.21199999999999999</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2019,13 +2019,13 @@
         <v>50</v>
       </c>
       <c r="B116">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="C116">
-        <v>0.27</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D116">
-        <v>-0.20399999999999999</v>
+        <v>-0.21199999999999999</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2033,13 +2033,13 @@
         <v>50</v>
       </c>
       <c r="B117">
-        <v>75000</v>
+        <v>15000</v>
       </c>
       <c r="C117">
-        <v>0.26600000000000001</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="D117">
-        <v>-0.19600000000000001</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2047,13 +2047,13 @@
         <v>50</v>
       </c>
       <c r="B118">
-        <v>100000</v>
+        <v>20000</v>
       </c>
       <c r="C118">
-        <v>0.25600000000000001</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="D118">
-        <v>-0.19</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2061,13 +2061,13 @@
         <v>50</v>
       </c>
       <c r="B119">
-        <v>200000</v>
+        <v>50000</v>
       </c>
       <c r="C119">
-        <v>0.20799999999999999</v>
+        <v>0.27</v>
       </c>
       <c r="D119">
-        <v>-0.14599999999999999</v>
+        <v>-0.20399999999999999</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2075,13 +2075,13 @@
         <v>50</v>
       </c>
       <c r="B120">
-        <v>300000</v>
+        <v>75000</v>
       </c>
       <c r="C120">
-        <v>0.16700000000000001</v>
+        <v>0.26600000000000001</v>
       </c>
       <c r="D120">
-        <v>-0.105</v>
+        <v>-0.19600000000000001</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2089,13 +2089,13 @@
         <v>50</v>
       </c>
       <c r="B121">
-        <v>400000</v>
+        <v>100000</v>
       </c>
       <c r="C121">
-        <v>0.13600000000000001</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="D121">
-        <v>-7.2999999999999995E-2</v>
+        <v>-0.19</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2103,13 +2103,13 @@
         <v>50</v>
       </c>
       <c r="B122">
-        <v>500000</v>
+        <v>200000</v>
       </c>
       <c r="C122">
-        <v>0.113</v>
+        <v>0.20799999999999999</v>
       </c>
       <c r="D122">
-        <v>-0.05</v>
+        <v>-0.14599999999999999</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2117,13 +2117,13 @@
         <v>50</v>
       </c>
       <c r="B123">
-        <v>600000</v>
+        <v>300000</v>
       </c>
       <c r="C123">
-        <v>9.8000000000000004E-2</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="D123">
-        <v>-3.3000000000000002E-2</v>
+        <v>-0.105</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2131,13 +2131,13 @@
         <v>50</v>
       </c>
       <c r="B124">
-        <v>700000</v>
+        <v>400000</v>
       </c>
       <c r="C124">
-        <v>8.6999999999999994E-2</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="D124">
-        <v>-2.1999999999999999E-2</v>
+        <v>-7.2999999999999995E-2</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2145,13 +2145,13 @@
         <v>50</v>
       </c>
       <c r="B125">
-        <v>750000</v>
+        <v>500000</v>
       </c>
       <c r="C125">
-        <v>8.2000000000000003E-2</v>
+        <v>0.113</v>
       </c>
       <c r="D125">
-        <v>-1.7000000000000001E-2</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2159,13 +2159,13 @@
         <v>50</v>
       </c>
       <c r="B126">
-        <v>800000</v>
+        <v>600000</v>
       </c>
       <c r="C126">
-        <v>7.9000000000000001E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="D126">
-        <v>-1.2999999999999999E-2</v>
+        <v>-3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2173,13 +2173,13 @@
         <v>50</v>
       </c>
       <c r="B127">
-        <v>900000</v>
+        <v>700000</v>
       </c>
       <c r="C127">
-        <v>7.1999999999999995E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="D127">
-        <v>-6.0000000000000001E-3</v>
+        <v>-2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2187,55 +2187,55 @@
         <v>50</v>
       </c>
       <c r="B128">
-        <v>1000000</v>
+        <v>750000</v>
       </c>
       <c r="C128">
-        <v>6.7000000000000004E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="D128">
-        <v>-2E-3</v>
+        <v>-1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B129">
-        <v>20</v>
+        <v>800000</v>
       </c>
       <c r="C129">
-        <v>0.54400000000000004</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="D129">
-        <v>-0.41599999999999998</v>
+        <v>-1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B130">
-        <v>100</v>
+        <v>900000</v>
       </c>
       <c r="C130">
-        <v>0.54800000000000004</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="D130">
-        <v>-0.42</v>
+        <v>-6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B131">
-        <v>200</v>
+        <v>1000000</v>
       </c>
       <c r="C131">
-        <v>0.54800000000000004</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="D131">
-        <v>-0.42</v>
+        <v>-2E-3</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2243,13 +2243,13 @@
         <v>100</v>
       </c>
       <c r="B132">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="C132">
-        <v>0.54800000000000004</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="D132">
-        <v>-0.42</v>
+        <v>-0.41599999999999998</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2257,13 +2257,13 @@
         <v>100</v>
       </c>
       <c r="B133">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C133">
-        <v>0.54400000000000004</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="D133">
-        <v>-0.42399999999999999</v>
+        <v>-0.42</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -2271,13 +2271,13 @@
         <v>100</v>
       </c>
       <c r="B134">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="C134">
-        <v>0.54400000000000004</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="D134">
-        <v>-0.42399999999999999</v>
+        <v>-0.42</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -2285,13 +2285,13 @@
         <v>100</v>
       </c>
       <c r="B135">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="C135">
-        <v>0.54400000000000004</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="D135">
-        <v>-0.42399999999999999</v>
+        <v>-0.42</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -2299,7 +2299,7 @@
         <v>100</v>
       </c>
       <c r="B136">
-        <v>7500</v>
+        <v>1000</v>
       </c>
       <c r="C136">
         <v>0.54400000000000004</v>
@@ -2313,13 +2313,13 @@
         <v>100</v>
       </c>
       <c r="B137">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="C137">
         <v>0.54400000000000004</v>
       </c>
       <c r="D137">
-        <v>-0.42</v>
+        <v>-0.42399999999999999</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -2327,13 +2327,13 @@
         <v>100</v>
       </c>
       <c r="B138">
-        <v>15000</v>
+        <v>5000</v>
       </c>
       <c r="C138">
         <v>0.54400000000000004</v>
       </c>
       <c r="D138">
-        <v>-0.42</v>
+        <v>-0.42399999999999999</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -2341,13 +2341,13 @@
         <v>100</v>
       </c>
       <c r="B139">
-        <v>20000</v>
+        <v>7500</v>
       </c>
       <c r="C139">
-        <v>0.54</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="D139">
-        <v>-0.41199999999999998</v>
+        <v>-0.42399999999999999</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -2355,13 +2355,13 @@
         <v>100</v>
       </c>
       <c r="B140">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="C140">
-        <v>0.5</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="D140">
-        <v>-0.376</v>
+        <v>-0.42</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -2369,13 +2369,13 @@
         <v>100</v>
       </c>
       <c r="B141">
-        <v>75000</v>
+        <v>15000</v>
       </c>
       <c r="C141">
-        <v>0.45600000000000002</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="D141">
-        <v>-0.33200000000000002</v>
+        <v>-0.42</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -2383,13 +2383,13 @@
         <v>100</v>
       </c>
       <c r="B142">
-        <v>100000</v>
+        <v>20000</v>
       </c>
       <c r="C142">
-        <v>0.41599999999999998</v>
+        <v>0.54</v>
       </c>
       <c r="D142">
-        <v>-0.28799999999999998</v>
+        <v>-0.41199999999999998</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -2397,13 +2397,13 @@
         <v>100</v>
       </c>
       <c r="B143">
-        <v>150000</v>
+        <v>50000</v>
       </c>
       <c r="C143">
-        <v>0.34799999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="D143">
-        <v>-0.216</v>
+        <v>-0.376</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -2411,13 +2411,13 @@
         <v>100</v>
       </c>
       <c r="B144">
-        <v>200000</v>
+        <v>75000</v>
       </c>
       <c r="C144">
-        <v>0.29199999999999998</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="D144">
-        <v>-0.16400000000000001</v>
+        <v>-0.33200000000000002</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -2425,13 +2425,13 @@
         <v>100</v>
       </c>
       <c r="B145">
-        <v>300000</v>
+        <v>100000</v>
       </c>
       <c r="C145">
-        <v>0.22</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="D145">
-        <v>-0.09</v>
+        <v>-0.28799999999999998</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -2439,13 +2439,13 @@
         <v>100</v>
       </c>
       <c r="B146">
-        <v>500000</v>
+        <v>150000</v>
       </c>
       <c r="C146">
-        <v>0.156</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="D146">
-        <v>-2.5999999999999999E-2</v>
+        <v>-0.216</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -2453,13 +2453,13 @@
         <v>100</v>
       </c>
       <c r="B147">
-        <v>600000</v>
+        <v>200000</v>
       </c>
       <c r="C147">
-        <v>0.13400000000000001</v>
+        <v>0.29199999999999998</v>
       </c>
       <c r="D147">
-        <v>-8.0000000000000002E-3</v>
+        <v>-0.16400000000000001</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -2467,13 +2467,13 @@
         <v>100</v>
       </c>
       <c r="B148">
-        <v>700000</v>
+        <v>300000</v>
       </c>
       <c r="C148">
-        <v>0.124</v>
+        <v>0.22</v>
       </c>
       <c r="D148">
-        <v>5.0000000000000001E-3</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -2481,55 +2481,55 @@
         <v>100</v>
       </c>
       <c r="B149">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="C149">
-        <v>0.10299999999999999</v>
+        <v>0.156</v>
       </c>
       <c r="D149">
-        <v>2.7E-2</v>
+        <v>-2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B150">
-        <v>20</v>
+        <v>600000</v>
       </c>
       <c r="C150">
-        <v>1.1000000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="D150">
-        <v>-0.84</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B151">
-        <v>100</v>
+        <v>700000</v>
       </c>
       <c r="C151">
-        <v>1.1000000000000001</v>
+        <v>0.124</v>
       </c>
       <c r="D151">
-        <v>-0.85</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B152">
-        <v>200</v>
+        <v>1000000</v>
       </c>
       <c r="C152">
-        <v>1.1000000000000001</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="D152">
-        <v>-0.85</v>
+        <v>2.7E-2</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -2537,13 +2537,13 @@
         <v>200</v>
       </c>
       <c r="B153">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="C153">
         <v>1.1000000000000001</v>
       </c>
       <c r="D153">
-        <v>-0.85</v>
+        <v>-0.84</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -2551,7 +2551,7 @@
         <v>200</v>
       </c>
       <c r="B154">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C154">
         <v>1.1000000000000001</v>
@@ -2565,13 +2565,13 @@
         <v>200</v>
       </c>
       <c r="B155">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="C155">
-        <v>1.1200000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D155">
-        <v>-0.87</v>
+        <v>-0.85</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -2579,13 +2579,13 @@
         <v>200</v>
       </c>
       <c r="B156">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="C156">
-        <v>1.1200000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D156">
-        <v>-0.87</v>
+        <v>-0.85</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -2593,13 +2593,13 @@
         <v>200</v>
       </c>
       <c r="B157">
-        <v>7500</v>
+        <v>1000</v>
       </c>
       <c r="C157">
-        <v>1.1200000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D157">
-        <v>-0.87</v>
+        <v>-0.85</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -2607,13 +2607,13 @@
         <v>200</v>
       </c>
       <c r="B158">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="C158">
-        <v>1.1000000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="D158">
-        <v>-0.85</v>
+        <v>-0.87</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -2621,13 +2621,13 @@
         <v>200</v>
       </c>
       <c r="B159">
-        <v>15000</v>
+        <v>5000</v>
       </c>
       <c r="C159">
-        <v>1.08</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="D159">
-        <v>-0.82</v>
+        <v>-0.87</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -2635,13 +2635,13 @@
         <v>200</v>
       </c>
       <c r="B160">
-        <v>20000</v>
+        <v>7500</v>
       </c>
       <c r="C160">
-        <v>1.05</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="D160">
-        <v>-0.8</v>
+        <v>-0.87</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -2649,13 +2649,13 @@
         <v>200</v>
       </c>
       <c r="B161">
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="C161">
-        <v>0.98</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D161">
-        <v>-0.73</v>
+        <v>-0.85</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -2663,13 +2663,13 @@
         <v>200</v>
       </c>
       <c r="B162">
-        <v>40000</v>
+        <v>15000</v>
       </c>
       <c r="C162">
-        <v>0.91</v>
+        <v>1.08</v>
       </c>
       <c r="D162">
-        <v>-0.65</v>
+        <v>-0.82</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -2677,13 +2677,13 @@
         <v>200</v>
       </c>
       <c r="B163">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="C163">
-        <v>0.85</v>
+        <v>1.05</v>
       </c>
       <c r="D163">
-        <v>-0.59</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -2691,13 +2691,13 @@
         <v>200</v>
       </c>
       <c r="B164">
-        <v>75000</v>
+        <v>30000</v>
       </c>
       <c r="C164">
-        <v>0.7</v>
+        <v>0.98</v>
       </c>
       <c r="D164">
-        <v>-0.44</v>
+        <v>-0.73</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -2705,13 +2705,13 @@
         <v>200</v>
       </c>
       <c r="B165">
-        <v>100000</v>
+        <v>40000</v>
       </c>
       <c r="C165">
-        <v>0.57999999999999996</v>
+        <v>0.91</v>
       </c>
       <c r="D165">
-        <v>-0.32400000000000001</v>
+        <v>-0.65</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -2719,13 +2719,13 @@
         <v>200</v>
       </c>
       <c r="B166">
-        <v>200000</v>
+        <v>50000</v>
       </c>
       <c r="C166">
-        <v>0.38400000000000001</v>
+        <v>0.85</v>
       </c>
       <c r="D166">
-        <v>-0.124</v>
+        <v>-0.59</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -2733,13 +2733,13 @@
         <v>200</v>
       </c>
       <c r="B167">
-        <v>500000</v>
+        <v>75000</v>
       </c>
       <c r="C167">
-        <v>0.224</v>
+        <v>0.7</v>
       </c>
       <c r="D167">
-        <v>3.4000000000000002E-2</v>
+        <v>-0.44</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -2747,13 +2747,13 @@
         <v>200</v>
       </c>
       <c r="B168">
-        <v>700000</v>
+        <v>100000</v>
       </c>
       <c r="C168">
-        <v>0.2</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D168">
-        <v>6.8000000000000005E-2</v>
+        <v>-0.32400000000000001</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -2761,12 +2761,54 @@
         <v>200</v>
       </c>
       <c r="B169">
+        <v>200000</v>
+      </c>
+      <c r="C169">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="D169">
+        <v>-0.124</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>200</v>
+      </c>
+      <c r="B170">
+        <v>500000</v>
+      </c>
+      <c r="C170">
+        <v>0.224</v>
+      </c>
+      <c r="D170">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>200</v>
+      </c>
+      <c r="B171">
+        <v>700000</v>
+      </c>
+      <c r="C171">
+        <v>0.2</v>
+      </c>
+      <c r="D171">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>200</v>
+      </c>
+      <c r="B172">
         <v>1000000</v>
       </c>
-      <c r="C169">
+      <c r="C172">
         <v>0.17299999999999999</v>
       </c>
-      <c r="D169">
+      <c r="D172">
         <v>8.8999999999999996E-2</v>
       </c>
     </row>

</xml_diff>